<commit_message>
updating multisensory stimulus generation
</commit_message>
<xml_diff>
--- a/meeting_and_analysis/20160801/multisensory_combos.xlsx
+++ b/meeting_and_analysis/20160801/multisensory_combos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t xml:space="preserve">dark </t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>legal trials</t>
+  </si>
+  <si>
+    <t>cool</t>
   </si>
 </sst>
 </file>
@@ -115,13 +118,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -476,22 +482,23 @@
     <col min="6" max="6" width="9.1640625" customWidth="1"/>
     <col min="7" max="7" width="8.5" customWidth="1"/>
     <col min="8" max="8" width="9.83203125" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="9" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:13">
+      <c r="C1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="5" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -515,59 +522,67 @@
       <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="5"/>
+      <c r="J2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="6"/>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="2"/>
+      <c r="L3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="5"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="2"/>
+      <c r="L4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:13">
+      <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="5"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="6"/>
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="5"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="5"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="6"/>
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
@@ -577,8 +592,8 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="5"/>
+    <row r="9" spans="1:13">
+      <c r="A9" s="6"/>
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
@@ -588,14 +603,22 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:13">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="C1:I1"/>
-    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>